<commit_message>
chore: publish messagedefinitions IG 1.0.1-trial-use
</commit_message>
<xml_diff>
--- a/ig/messagedefinitions/StructureDefinition-medcom-messaging-messagedefinition-fhir.xlsx
+++ b/ig/messagedefinitions/StructureDefinition-medcom-messaging-messagedefinition-fhir.xlsx
@@ -33,7 +33,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.0.0-trial-use</t>
+    <t>1.0.1-trial-use</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-06-30T11:03:09+00:00</t>
+    <t>2025-09-17T09:43:38+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
chore: publish messagedefinitions IG 1.0.1-trial-use (#31)
Co-authored-by: olw-medcom <olw-medcom@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/ig/messagedefinitions/StructureDefinition-medcom-messaging-messagedefinition-fhir.xlsx
+++ b/ig/messagedefinitions/StructureDefinition-medcom-messaging-messagedefinition-fhir.xlsx
@@ -33,7 +33,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.0.0-trial-use</t>
+    <t>1.0.1-trial-use</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-06-30T11:03:09+00:00</t>
+    <t>2025-09-17T09:43:38+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>